<commit_message>
Publish documentation 0.1.1, ror 0.1.1, annuaire 1.0.0-ballot (#23)
* add documentation script

* publish documentation 0.1.1

* publish ror 0.1.1

* add annuaire package-feed

* publish annuaire ballot
</commit_message>
<xml_diff>
--- a/www/ig/fhir/ror/CodeSystem-input-task-ror-codesystem.xlsx
+++ b/www/ig/fhir/ror/CodeSystem-input-task-ror-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>0.1.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-04-12T17:55:39+02:00</t>
+    <t>2023-06-02T12:02:38+02:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>